<commit_message>
files now are passed into command line
</commit_message>
<xml_diff>
--- a/PM.xlsx
+++ b/PM.xlsx
@@ -245,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -257,12 +257,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -334,23 +339,26 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1602,7 +1610,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1736,10 +1744,10 @@
       <c r="F2" t="s" s="3">
         <v>30</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" t="s" s="3">
         <v>31</v>
       </c>
@@ -1790,392 +1798,308 @@
       </c>
     </row>
     <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="5">
         <v>39</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="5">
         <v>40</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>2032193997</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="F3" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" t="s" s="4">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="L3" t="s" s="4">
+      <c r="L3" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="M3" t="s" s="4">
+      <c r="M3" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="5">
         <v>9</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="5">
         <v>8</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="5">
         <v>8</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="5">
         <v>10</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="5">
         <v>8</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="5">
         <v>9</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="5">
         <v>10</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="5">
         <v>9</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="5">
         <v>10</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="5">
         <v>9</v>
       </c>
-      <c r="X3" t="s" s="4">
+      <c r="X3" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="Y3" t="s" s="4">
+      <c r="Y3" t="s" s="5">
         <v>42</v>
       </c>
-      <c r="Z3" t="s" s="4">
+      <c r="Z3" t="s" s="5">
         <v>43</v>
       </c>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="A4" t="s" s="5">
         <v>44</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" t="s" s="5">
         <v>46</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" t="s" s="5">
         <v>47</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>553631759</v>
       </c>
-      <c r="F4" t="s" s="4">
+      <c r="F4" t="s" s="5">
         <v>48</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" t="s" s="4">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="L4" t="s" s="4">
+      <c r="L4" t="s" s="5">
         <v>49</v>
       </c>
-      <c r="M4" t="s" s="4">
+      <c r="M4" t="s" s="5">
         <v>50</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="5">
         <v>8</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="5">
         <v>5</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="5">
         <v>5</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="5">
         <v>10</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="5">
         <v>10</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="5">
         <v>3</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="5">
         <v>3</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="5">
         <v>5</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="5">
         <v>5</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="5">
         <v>4</v>
       </c>
-      <c r="X4" t="s" s="4">
+      <c r="X4" t="s" s="5">
         <v>51</v>
       </c>
-      <c r="Y4" t="s" s="4">
+      <c r="Y4" t="s" s="5">
         <v>52</v>
       </c>
-      <c r="Z4" t="s" s="4">
+      <c r="Z4" t="s" s="5">
         <v>53</v>
       </c>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="A5" t="s" s="5">
         <v>54</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" t="s" s="5">
         <v>55</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" t="s" s="5">
         <v>56</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>-1888203339</v>
       </c>
-      <c r="F5" t="s" s="4">
+      <c r="F5" t="s" s="5">
         <v>57</v>
       </c>
-      <c r="G5" t="s" s="4">
+      <c r="G5" t="s" s="5">
         <v>58</v>
       </c>
-      <c r="H5" t="s" s="4">
+      <c r="H5" t="s" s="5">
         <v>59</v>
       </c>
-      <c r="I5" t="s" s="4">
+      <c r="I5" t="s" s="5">
         <v>60</v>
       </c>
-      <c r="J5" t="s" s="4">
+      <c r="J5" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="K5" t="s" s="4">
+      <c r="K5" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="L5" t="s" s="4">
+      <c r="L5" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="M5" t="s" s="4">
+      <c r="M5" t="s" s="5">
         <v>49</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="5">
         <v>6</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="5">
         <v>8</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="5">
         <v>7</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="5">
         <v>9</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="5">
         <v>10</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="5">
         <v>7</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="5">
         <v>7</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="5">
         <v>8</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="5">
         <v>8</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5" s="5">
         <v>9</v>
       </c>
-      <c r="X5" t="s" s="4">
+      <c r="X5" t="s" s="5">
         <v>62</v>
       </c>
-      <c r="Y5" t="s" s="4">
+      <c r="Y5" t="s" s="5">
         <v>63</v>
       </c>
-      <c r="Z5" t="s" s="4">
+      <c r="Z5" t="s" s="5">
         <v>64</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="A6" t="s" s="5">
         <v>65</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="5">
         <v>66</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" t="s" s="5">
         <v>67</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" t="s" s="5">
         <v>68</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>-1890949374</v>
       </c>
-      <c r="F6" t="s" s="4">
+      <c r="F6" t="s" s="5">
         <v>57</v>
       </c>
-      <c r="G6" t="s" s="4">
+      <c r="G6" t="s" s="5">
         <v>69</v>
       </c>
-      <c r="H6" t="s" s="4">
+      <c r="H6" t="s" s="5">
         <v>70</v>
       </c>
-      <c r="I6" t="s" s="4">
+      <c r="I6" t="s" s="5">
         <v>71</v>
       </c>
-      <c r="J6" t="s" s="4">
+      <c r="J6" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="K6" t="s" s="4">
+      <c r="K6" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="L6" t="s" s="4">
+      <c r="L6" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="M6" t="s" s="4">
+      <c r="M6" t="s" s="5">
         <v>50</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="5">
         <v>8</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="5">
         <v>7</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="5">
         <v>5</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="5">
         <v>8</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="5">
         <v>9</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="5">
         <v>7</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="5">
         <v>7</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="5">
         <v>7</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="5">
         <v>10</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="5">
         <v>8</v>
       </c>
-      <c r="X6" t="s" s="4">
+      <c r="X6" t="s" s="5">
         <v>72</v>
       </c>
-      <c r="Y6" t="s" s="4">
+      <c r="Y6" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="Z6" t="s" s="4">
+      <c r="Z6" t="s" s="5">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-    </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>